<commit_message>
start add data in db
</commit_message>
<xml_diff>
--- a/documents/shoes.xlsx
+++ b/documents/shoes.xlsx
@@ -7,6 +7,7 @@
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr/>
   <extLst>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>№</t>
   </si>
@@ -171,6 +172,45 @@
   </si>
   <si>
     <t>ADYS100647-3BK</t>
+  </si>
+  <si>
+    <t>beige</t>
+  </si>
+  <si>
+    <t>beige-gum</t>
+  </si>
+  <si>
+    <t>black-brown</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>brown</t>
+  </si>
+  <si>
+    <t>brown-black</t>
+  </si>
+  <si>
+    <t>gray</t>
+  </si>
+  <si>
+    <t>grey</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>white</t>
+  </si>
+  <si>
+    <t>white-black</t>
+  </si>
+  <si>
+    <t>white-red</t>
+  </si>
+  <si>
+    <t>yellow</t>
   </si>
 </sst>
 </file>
@@ -226,12 +266,10 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -731,7 +769,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -739,7 +777,7 @@
   <cols>
     <col customWidth="1" min="2" max="2" width="15.00390625"/>
     <col bestFit="1" customWidth="1" min="4" max="4" width="52.140625"/>
-    <col bestFit="1" min="7" max="7" width="11.28125"/>
+    <col bestFit="1" min="7" max="7" width="11.7109375"/>
     <col bestFit="1" customWidth="1" min="8" max="8" width="60.57421875"/>
   </cols>
   <sheetData>
@@ -860,10 +898,10 @@
       <c r="D5" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="5" t="s">
+      <c r="E5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>12</v>
       </c>
       <c r="G5" s="2">
@@ -895,7 +933,7 @@
       <c r="G6" s="2">
         <v>6990</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="5" t="s">
         <v>26</v>
       </c>
     </row>
@@ -964,7 +1002,7 @@
       <c r="D9" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F9" s="4" t="s">
@@ -1113,4 +1151,117 @@
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="14.7109375"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.25">
+      <c r="A1" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25">
+      <c r="A2" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25">
+      <c r="A3" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="A4" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25">
+      <c r="A5" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="A6" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" ht="14.25">
+      <c r="A7" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" ht="14.25">
+      <c r="A8" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" ht="14.25">
+      <c r="A9" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" ht="14.25">
+      <c r="A10" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" ht="14.25">
+      <c r="A11" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" ht="14.25">
+      <c r="A12" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" ht="14.25">
+      <c r="A13" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" ht="14.25">
+      <c r="A14" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" ht="14.25">
+      <c r="A15" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" ht="14.25">
+      <c r="A16" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" ht="14.25">
+      <c r="A17" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" ht="14.25">
+      <c r="A18" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A1:A26" columnSort="0">
+    <sortCondition sortBy="value" descending="0" ref="A1:A26"/>
+  </sortState>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>